<commit_message>
Added the ability to disable synchronization. Fix in docs
</commit_message>
<xml_diff>
--- a/docs/Протокол/GyverLamp_UDP.xlsx
+++ b/docs/Протокол/GyverLamp_UDP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FeryaFox\Desktop\GyverLamp2Sync\docs\Протокол\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94757937-C100-4AA6-A324-1354774BCF6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C28AA3B8-A29D-4E22-A8A3-D243C56DE38D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24825" yWindow="21105" windowWidth="27045" windowHeight="19215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19245" yWindow="0" windowWidth="42285" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="169">
   <si>
     <t>Дата 0 (ключ GL)</t>
   </si>
@@ -524,6 +524,9 @@
   </si>
   <si>
     <t>6 - номер версии синхронизации</t>
+  </si>
+  <si>
+    <t>флаг на свою яркость</t>
   </si>
 </sst>
 </file>
@@ -867,8 +870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1508,7 +1511,7 @@
         <v>94</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>95</v>
+        <v>168</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>96</v>

</xml_diff>

<commit_message>
Fix sync Update Docs
</commit_message>
<xml_diff>
--- a/docs/Протокол/GyverLamp_UDP.xlsx
+++ b/docs/Протокол/GyverLamp_UDP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FeryaFox\Desktop\GyverLamp2Sync\docs\Протокол\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C28AA3B8-A29D-4E22-A8A3-D243C56DE38D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FADDC8-1389-4762-B30A-309DD60066C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19245" yWindow="0" windowWidth="42285" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30612" yWindow="4068" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -490,9 +490,6 @@
     <t>20 - синхронизация</t>
   </si>
   <si>
-    <t>RGL</t>
-  </si>
-  <si>
     <t>0 - настройки (RGL 0)</t>
   </si>
   <si>
@@ -527,6 +524,9 @@
   </si>
   <si>
     <t>флаг на свою яркость</t>
+  </si>
+  <si>
+    <t>GL_RESP</t>
   </si>
 </sst>
 </file>
@@ -871,7 +871,7 @@
   <dimension ref="A1:AE62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1511,7 +1511,7 @@
         <v>94</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>96</v>
@@ -1938,7 +1938,7 @@
         <v>155</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
@@ -1960,7 +1960,7 @@
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
@@ -1982,7 +1982,7 @@
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
@@ -2004,7 +2004,7 @@
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
@@ -2027,7 +2027,7 @@
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
@@ -2050,7 +2050,7 @@
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
@@ -2092,7 +2092,7 @@
     <row r="36" spans="1:31" ht="30" customHeight="1">
       <c r="A36" s="3"/>
       <c r="B36" s="3" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
       <c r="C36" s="3">
         <v>0</v>
@@ -2113,13 +2113,13 @@
         <v>40</v>
       </c>
       <c r="I36" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="J36" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="J36" s="3" t="s">
+      <c r="K36" s="3" t="s">
         <v>159</v>
-      </c>
-      <c r="K36" s="3" t="s">
-        <v>160</v>
       </c>
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
@@ -2334,7 +2334,7 @@
         <v>2</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>93</v>
@@ -2543,7 +2543,7 @@
         <v>138</v>
       </c>
       <c r="AA44" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AB44" s="3" t="s">
         <v>30</v>

</xml_diff>